<commit_message>
add parallel and logs to testsEnable parallel test execution and add logging
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
   <si>
     <t>First name</t>
   </si>
@@ -301,6 +301,30 @@
   </si>
   <si>
     <t>000054176</t>
+  </si>
+  <si>
+    <t>000054816</t>
+  </si>
+  <si>
+    <t>000054817</t>
+  </si>
+  <si>
+    <t>000054818</t>
+  </si>
+  <si>
+    <t>000054819</t>
+  </si>
+  <si>
+    <t>000054865</t>
+  </si>
+  <si>
+    <t>000054866</t>
+  </si>
+  <si>
+    <t>000054890</t>
+  </si>
+  <si>
+    <t>000054891</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1477,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A26"/>
@@ -1484,6 +1508,46 @@
         <v>91</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Enable parallel test execution and add logging
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
   <si>
     <t>First name</t>
   </si>
@@ -301,6 +301,30 @@
   </si>
   <si>
     <t>000054176</t>
+  </si>
+  <si>
+    <t>000054816</t>
+  </si>
+  <si>
+    <t>000054817</t>
+  </si>
+  <si>
+    <t>000054818</t>
+  </si>
+  <si>
+    <t>000054819</t>
+  </si>
+  <si>
+    <t>000054865</t>
+  </si>
+  <si>
+    <t>000054866</t>
+  </si>
+  <si>
+    <t>000054890</t>
+  </si>
+  <si>
+    <t>000054891</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1477,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A26"/>
@@ -1484,6 +1508,46 @@
         <v>91</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>